<commit_message>
Changes done in My Listeners For all the 3 Scenarios
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_2_3_TestData.xlsx
+++ b/testdata/Scenario1_2_3_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408439\CTS_Java_Training\Practicals\IntelliJ_Selenium_Projects\Hackathon_Project\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580E5308-3765-41D9-896E-34B2C5BB0322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66424C1-1D16-4238-8481-B2FED71CC54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="81">
   <si>
     <t>TC_ID</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>TC_003_04</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>15</t>
@@ -288,7 +285,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -356,6 +352,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,22 +689,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3050-D1DC-49F4-900E-5DA4D3857D18}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0"/>
-    <col min="2" max="2" customWidth="true" width="10.36328125"/>
-    <col min="3" max="3" customWidth="true" width="42.6328125"/>
-    <col min="4" max="4" customWidth="true" width="13.1796875"/>
-    <col min="5" max="5" customWidth="true" width="48.1796875"/>
-    <col min="6" max="6" customWidth="true" width="18.90625"/>
-    <col min="7" max="7" customWidth="true" width="12.7265625"/>
-    <col min="8" max="8" customWidth="true" width="19.6328125"/>
-    <col min="9" max="9" customWidth="true" width="10.26953125"/>
-    <col min="10" max="11" customWidth="true" width="11.08984375"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="42.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="48.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+    <col min="10" max="11" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -749,16 +746,16 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>
@@ -768,62 +765,64 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s" s="0">
+      <c r="L3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" t="s" s="0">
+      <c r="L4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -835,31 +834,31 @@
       <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L5" t="s" s="0">
+      <c r="L5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
@@ -867,31 +866,31 @@
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L6" t="s" s="0">
+      <c r="L6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s" s="0">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
@@ -899,34 +898,34 @@
       <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" t="s" s="0">
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="L7" t="s" s="0">
+      <c r="L7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s" s="0">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -934,34 +933,34 @@
       <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s" s="0">
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
@@ -969,76 +968,76 @@
       <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" t="s" s="0">
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="L9" t="s" s="0">
+      <c r="L9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" t="s" s="0">
+      <c r="H10" t="s">
         <v>22</v>
       </c>
-      <c r="L10" t="s" s="0">
+      <c r="L10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s" s="0">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="L11" t="s" s="0">
+      <c r="L11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s" s="0">
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1047,254 +1046,260 @@
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s" s="0">
+      <c r="H12" t="s">
         <v>26</v>
       </c>
-      <c r="L12" t="s" s="0">
+      <c r="L12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L13" t="s" s="0">
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="L14" t="s" s="0">
+      <c r="L14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="L15" t="s" s="0">
+      <c r="L15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s" s="0">
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L16" t="s" s="0">
+      <c r="L16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s" s="0">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G17" t="s" s="0">
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="L17" t="s" s="0">
+      <c r="L17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
         <v>47</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G18" t="s" s="0">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s" s="0">
+      <c r="H18" t="s">
         <v>53</v>
       </c>
-      <c r="L18" t="s" s="0">
+      <c r="L18" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s" s="0">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s" s="0">
+      <c r="G19" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="s" s="0">
+      <c r="H19" t="s">
         <v>53</v>
       </c>
-      <c r="I19" t="s" s="0">
+      <c r="I19" t="s">
         <v>55</v>
       </c>
-      <c r="L19" t="s" s="0">
+      <c r="L19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s" s="0">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G20" t="s" s="0">
+      <c r="G20" t="s">
         <v>51</v>
       </c>
-      <c r="H20" t="s" s="0">
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="I20" t="s" s="0">
+      <c r="I20" t="s">
         <v>55</v>
       </c>
-      <c r="J20" t="s" s="0">
+      <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L20" t="s" s="0">
-        <v>77</v>
+      <c r="L20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="F21" s="2"/>
       <c r="K21" s="2"/>
+      <c r="L21" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="2"/>
       <c r="K22" s="2"/>
+      <c r="L22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1306,22 +1311,25 @@
       <c r="E23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L23" t="s" s="0">
+      <c r="L23" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" t="s" s="0">
-        <v>81</v>
+      <c r="B24" t="s">
+        <v>80</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" t="s" s="0">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel to cucumber but only for scenario 1
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_2_3_TestData.xlsx
+++ b/testdata/Scenario1_2_3_TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408439\CTS_Java_Training\Practicals\IntelliJ_Selenium_Projects\Hackathon_Project\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66424C1-1D16-4238-8481-B2FED71CC54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BB1DD3-55DA-4886-AF5A-E2CEFC71638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="82">
   <si>
     <t>TC_ID</t>
   </si>
@@ -269,26 +269,25 @@
     <t>TC_003_04</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>validateRetrievingHealthInsuranceData</t>
   </si>
   <si>
     <t>TC_003_05</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Test Data8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -356,7 +355,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,27 +689,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDE3050-D1DC-49F4-900E-5DA4D3857D18}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0"/>
-    <col min="2" max="2" customWidth="true" width="10.36328125"/>
-    <col min="3" max="3" customWidth="true" width="42.6328125"/>
-    <col min="4" max="4" customWidth="true" width="13.1796875"/>
-    <col min="5" max="5" customWidth="true" width="48.1796875"/>
-    <col min="6" max="6" customWidth="true" width="18.90625"/>
-    <col min="7" max="7" customWidth="true" width="12.7265625"/>
-    <col min="8" max="8" customWidth="true" width="19.6328125"/>
-    <col min="9" max="9" customWidth="true" width="10.26953125"/>
-    <col min="10" max="11" customWidth="true" width="11.08984375"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="42.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="5" max="5" width="48.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.08984375" customWidth="1"/>
+    <col min="10" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -746,20 +745,23 @@
         <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>
@@ -769,100 +771,101 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="L2" s="1"/>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
+      <c r="D4" t="s">
+        <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L5" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
@@ -870,31 +873,31 @@
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L6" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s" s="0">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
@@ -902,34 +905,34 @@
       <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" t="s" s="0">
+      <c r="K7" t="s">
         <v>18</v>
       </c>
-      <c r="L7" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s" s="0">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -937,34 +940,34 @@
       <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s" s="0">
+      <c r="K8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
@@ -972,338 +975,341 @@
       <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" t="s" s="0">
+      <c r="K9" t="s">
         <v>18</v>
       </c>
-      <c r="L9" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="L10" t="s">
         <v>22</v>
       </c>
-      <c r="L10" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s" s="0">
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="L11" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+      <c r="M11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s" s="0">
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s" s="0">
+      <c r="L12" t="s">
         <v>26</v>
       </c>
-      <c r="L12" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+      <c r="M12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L13" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="L14" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+      <c r="M14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="L15" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" t="s" s="0">
+      <c r="M15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s" s="0">
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L16" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
+      <c r="M16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s" s="0">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G17" t="s" s="0">
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="L17" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+      <c r="M17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
         <v>47</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G18" t="s" s="0">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s" s="0">
+      <c r="H18" t="s">
         <v>53</v>
       </c>
-      <c r="L18" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+      <c r="M18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s" s="0">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s" s="0">
+      <c r="G19" t="s">
         <v>51</v>
       </c>
-      <c r="H19" t="s" s="0">
+      <c r="H19" t="s">
         <v>53</v>
       </c>
-      <c r="I19" t="s" s="0">
+      <c r="I19" t="s">
         <v>55</v>
       </c>
-      <c r="L19" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+      <c r="M19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s" s="0">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G20" t="s" s="0">
+      <c r="G20" t="s">
         <v>51</v>
       </c>
-      <c r="H20" t="s" s="0">
+      <c r="H20" t="s">
         <v>53</v>
       </c>
-      <c r="I20" t="s" s="0">
+      <c r="I20" t="s">
         <v>55</v>
       </c>
-      <c r="J20" t="s" s="0">
+      <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L20" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+      <c r="L20" s="2"/>
+      <c r="M20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
       <c r="F21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+      <c r="L21" s="2"/>
+      <c r="M21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s" s="0">
+      <c r="L22" s="2"/>
+      <c r="M22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1315,24 +1321,24 @@
       <c r="E23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L23" t="s" s="0">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" t="s" s="0">
+      <c r="M23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" t="s" s="0">
-        <v>80</v>
+      <c r="B24" t="s">
+        <v>78</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L24" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Getting data from excel for scenario1 bdd
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_2_3_TestData.xlsx
+++ b/testdata/Scenario1_2_3_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408439\CTS_Java_Training\Practicals\IntelliJ_Selenium_Projects\Hackathon_Project\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BB1DD3-55DA-4886-AF5A-E2CEFC71638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75010A-7A96-4285-8797-01C497AC8510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -275,13 +275,13 @@
     <t>TC_003_05</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Test Data8</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -692,7 +692,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,7 +745,7 @@
         <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>28</v>
@@ -810,10 +810,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M4" t="s">
         <v>70</v>
@@ -862,10 +862,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
@@ -894,10 +894,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
@@ -929,10 +929,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -964,10 +964,10 @@
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
@@ -999,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L10" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Scenario1 BDD Completed By Vedant Adka
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_2_3_TestData.xlsx
+++ b/testdata/Scenario1_2_3_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2408439\CTS_Java_Training\Practicals\IntelliJ_Selenium_Projects\Hackathon_Project\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75010A-7A96-4285-8797-01C497AC8510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0438A9D7-BFFA-44FE-81E2-E695F6808295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE57E9C9-A6C1-4A7D-85B9-1309751074B4}"/>
   </bookViews>
@@ -692,7 +692,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>